<commit_message>
waiting for other information
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\clients\Klinge Corp\SIP\SIPV8\Export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3EE798-2E2D-4D2F-B9ED-7EAEE4544591}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF7854D1-7F33-4501-83AE-727A5FC1FBCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15075" yWindow="2130" windowWidth="10050" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>CONTNUM</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>332439</t>
+  </si>
+  <si>
+    <t>SIN1</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -839,7 +844,12 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="1">
+        <v>332439</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>